<commit_message>
added battery management parts
</commit_message>
<xml_diff>
--- a/Projects/Power Management Tester/Battery Management BOM.xlsx
+++ b/Projects/Power Management Tester/Battery Management BOM.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21721"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="100" yWindow="80" windowWidth="25600" windowHeight="14680" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14760" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="100">
   <si>
     <t>Schematic Ref.</t>
   </si>
@@ -255,15 +255,6 @@
     <t>U2</t>
   </si>
   <si>
-    <t>voltage reg</t>
-  </si>
-  <si>
-    <t>LM2623</t>
-  </si>
-  <si>
-    <t>U3</t>
-  </si>
-  <si>
     <t>2k</t>
   </si>
   <si>
@@ -310,6 +301,24 @@
   </si>
   <si>
     <t>LED1, LED2</t>
+  </si>
+  <si>
+    <t>1175-1015-ND</t>
+  </si>
+  <si>
+    <t>1002-001-01000</t>
+  </si>
+  <si>
+    <t>CNC Tech</t>
+  </si>
+  <si>
+    <t>USB receptacle</t>
+  </si>
+  <si>
+    <t>K1, K3</t>
+  </si>
+  <si>
+    <t>(alt) means it has the same footprint and we can test it as an alternative part</t>
   </si>
 </sst>
 </file>
@@ -742,10 +751,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M22"/>
+  <dimension ref="A1:M25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="K26" sqref="K26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -755,7 +764,7 @@
     <col min="5" max="5" width="18.5" customWidth="1"/>
     <col min="6" max="6" width="16.1640625" style="6" customWidth="1"/>
     <col min="7" max="7" width="33.5" customWidth="1"/>
-    <col min="8" max="8" width="20.83203125" customWidth="1"/>
+    <col min="8" max="8" width="24.5" customWidth="1"/>
     <col min="10" max="10" width="26" customWidth="1"/>
     <col min="11" max="11" width="13" customWidth="1"/>
   </cols>
@@ -772,7 +781,7 @@
     </row>
     <row r="3" spans="1:13">
       <c r="A3" s="3">
-        <v>41251</v>
+        <v>41289</v>
       </c>
     </row>
     <row r="6" spans="1:13">
@@ -824,7 +833,7 @@
         <v>17</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="H7" s="4" t="s">
         <v>19</v>
@@ -1136,7 +1145,7 @@
     </row>
     <row r="16" spans="1:13">
       <c r="C16" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D16" t="s">
         <v>72</v>
@@ -1181,19 +1190,19 @@
         <v>20</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="I17" t="s">
         <v>12</v>
       </c>
       <c r="J17" s="5" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="K17">
         <v>1</v>
@@ -1204,25 +1213,25 @@
         <v>62</v>
       </c>
       <c r="D18" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E18" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F18" s="6" t="s">
         <v>61</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="I18" t="s">
         <v>12</v>
       </c>
       <c r="J18" s="5" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="K18">
         <v>1</v>
@@ -1237,7 +1246,7 @@
     </row>
     <row r="19" spans="3:13">
       <c r="C19" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D19" t="s">
         <v>47</v>
@@ -1252,13 +1261,13 @@
         <v>75</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="I19" t="s">
         <v>12</v>
       </c>
       <c r="J19" s="5" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="K19">
         <v>1</v>
@@ -1269,10 +1278,10 @@
     </row>
     <row r="20" spans="3:13">
       <c r="C20" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D20" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E20" s="8">
         <v>470</v>
@@ -1281,43 +1290,57 @@
         <v>61</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="H20" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="I20" t="s">
+        <v>12</v>
+      </c>
+      <c r="J20" s="5" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="21" spans="3:13">
+      <c r="C21" t="s">
+        <v>98</v>
+      </c>
+      <c r="D21" t="s">
+        <v>97</v>
+      </c>
+      <c r="E21" t="s">
+        <v>20</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="G21" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="H21" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="I20" t="s">
-        <v>12</v>
-      </c>
-      <c r="J20" s="5" t="s">
+      <c r="I21" t="s">
+        <v>12</v>
+      </c>
+      <c r="J21" s="5" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="22" spans="3:13">
-      <c r="C22" t="s">
-        <v>80</v>
-      </c>
-      <c r="D22" t="s">
-        <v>78</v>
-      </c>
-      <c r="E22" t="s">
-        <v>79</v>
-      </c>
-      <c r="F22" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="I22" t="s">
-        <v>12</v>
-      </c>
-      <c r="K22">
-        <v>1</v>
-      </c>
-      <c r="L22">
-        <v>1.52</v>
-      </c>
-      <c r="M22">
-        <f>K22*L22</f>
-        <v>1.52</v>
+      <c r="K21">
+        <v>2</v>
+      </c>
+      <c r="L21">
+        <v>0.69</v>
+      </c>
+      <c r="M21">
+        <f t="shared" ref="M21" si="1">K21*L21</f>
+        <v>1.38</v>
+      </c>
+    </row>
+    <row r="25" spans="3:13">
+      <c r="C25" t="s">
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -1349,6 +1372,8 @@
     <hyperlink ref="G19" r:id="rId25"/>
     <hyperlink ref="J20" r:id="rId26"/>
     <hyperlink ref="G20" r:id="rId27"/>
+    <hyperlink ref="J21" r:id="rId28"/>
+    <hyperlink ref="G21" r:id="rId29"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>